<commit_message>
Fixed the bug where the ui path assistant didn't have correct file path
</commit_message>
<xml_diff>
--- a/sitrep_data.xlsx
+++ b/sitrep_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\Desktop\ITSOLUTIONS\itsolutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228A8FDF-5D57-45F9-BA15-6375C453D818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EBCDFB-6F95-4963-A064-B18054ABC3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2790" windowWidth="29040" windowHeight="15840" xr2:uid="{E7EB22A9-ED07-4AC3-B6A9-C8759CBF059F}"/>
+    <workbookView xWindow="-27420" yWindow="7425" windowWidth="21600" windowHeight="11385" xr2:uid="{E7EB22A9-ED07-4AC3-B6A9-C8759CBF059F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sitreps" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,218 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="70">
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Incident</t>
+  </si>
+  <si>
+    <t>DateOf</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Offender</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Alcohol</t>
+  </si>
+  <si>
+    <t>Drugs</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>sitrep</t>
+  </si>
+  <si>
+    <t>RACE DISCRIMINATION_x000D_</t>
+  </si>
+  <si>
+    <t>2021-06-15 10:28:41.078578_x000D_</t>
+  </si>
+  <si>
+    <t>University of Texas Longhorns_x000D_</t>
+  </si>
+  <si>
+    <t>O-6_x000D_</t>
+  </si>
+  <si>
+    <t>MALE_x000D_</t>
+  </si>
+  <si>
+    <t>30_x000D_</t>
+  </si>
+  <si>
+    <t>CAUCASIAN_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NO_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Incident occured on 2021-06-15 10:28:41.078578 at University of Texas Longhorns with O-6</t>
+  </si>
+  <si>
+    <t>2021-06-15 10:28:52.596080_x000D_</t>
+  </si>
+  <si>
+    <t>CIV_x000D_</t>
+  </si>
+  <si>
+    <t>FEMALE_x000D_</t>
+  </si>
+  <si>
+    <t>39_x000D_</t>
+  </si>
+  <si>
+    <t>WITHHELD_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Incident occured on 2021-06-15 10:28:52.596080 at University of Texas Longhorns with CIV</t>
+  </si>
+  <si>
+    <t>SEXUAL ASSAULT_x000D_</t>
+  </si>
+  <si>
+    <t>2021-06-15 10:29:04.037113_x000D_</t>
+  </si>
+  <si>
+    <t>Dallas Cowboys_x000D_</t>
+  </si>
+  <si>
+    <t>E-2_x000D_</t>
+  </si>
+  <si>
+    <t>19_x000D_</t>
+  </si>
+  <si>
+    <t>AFRICAN-AMERICAN_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Incident occured on 2021-06-15 10:29:04.037113 at Dallas Cowboys with E-2</t>
+  </si>
+  <si>
+    <t>DOMESTIC ABUSE_x000D_</t>
+  </si>
+  <si>
+    <t>2021-06-15 10:29:15.075038_x000D_</t>
+  </si>
+  <si>
+    <t>San Antonio Spurs_x000D_</t>
+  </si>
+  <si>
+    <t>E-3_x000D_</t>
+  </si>
+  <si>
+    <t>35_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Incident occured on 2021-06-15 10:29:15.075038 at San Antonio Spurs with E-3</t>
+  </si>
+  <si>
+    <t>2021-06-15 10:29:26.072398_x000D_</t>
+  </si>
+  <si>
+    <t>O-4_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Incident occured on 2021-06-15 10:29:26.072398 at San Antonio Spurs with O-4</t>
+  </si>
+  <si>
+    <t>2021-06-15 10:29:37.054628_x000D_</t>
+  </si>
+  <si>
+    <t>31_x000D_</t>
+  </si>
+  <si>
+    <t>OTHER_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YES_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Incident occured on 2021-06-15 10:29:37.054628 at University of Texas Longhorns with E-3</t>
+  </si>
+  <si>
+    <t>VEHICULAR ACCIDENT_x000D_</t>
+  </si>
+  <si>
+    <t>2021-06-15 10:29:48.160535_x000D_</t>
+  </si>
+  <si>
+    <t>O-9_x000D_</t>
+  </si>
+  <si>
+    <t>43_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Incident occured on 2021-06-15 10:29:48.160535 at San Antonio Spurs with O-9</t>
+  </si>
+  <si>
+    <t>GENDER DISCRIMINATION_x000D_</t>
+  </si>
+  <si>
+    <t>2021-06-15 10:29:59.063641_x000D_</t>
+  </si>
+  <si>
+    <t>New York Yankees_x000D_</t>
+  </si>
+  <si>
+    <t>O-3_x000D_</t>
+  </si>
+  <si>
+    <t>32_x000D_</t>
+  </si>
+  <si>
+    <t>ASIAN_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Incident occured on 2021-06-15 10:29:59.063641 at New York Yankees with O-3</t>
+  </si>
+  <si>
+    <t>2021-06-15 10:30:10.084966_x000D_</t>
+  </si>
+  <si>
+    <t>28_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Incident occured on 2021-06-15 10:30:10.084966 at San Antonio Spurs with O-6</t>
+  </si>
+  <si>
+    <t>2021-06-15 10:30:21.607550_x000D_</t>
+  </si>
+  <si>
+    <t>O-8_x000D_</t>
+  </si>
+  <si>
+    <t>52_x000D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Incident occured on 2021-06-15 10:30:21.607550 at University of Texas Longhorns with O-8</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA72F7DB-2098-431E-AF94-0FE573276EF5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,8 +612,428 @@
     <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="121.85546875" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>